<commit_message>
completed Past teaching story
</commit_message>
<xml_diff>
--- a/assets/story/opening.xlsx
+++ b/assets/story/opening.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\เบ็ดเตล็ด\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\OneDrive\เอกสาร\GitHub\testgame\assets\story\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929F8970-72EB-4D0F-8DD0-50DEF2E1F8B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDC003F-6C96-4D4B-8CA8-1E94760ED608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{B095E92E-D879-4822-87EF-4147D0100398}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B095E92E-D879-4822-87EF-4147D0100398}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>conversation</t>
-  </si>
-  <si>
     <t>Narrator</t>
   </si>
   <si>
@@ -120,6 +117,12 @@
   </si>
   <si>
     <t>Past,Present,Future</t>
+  </si>
+  <si>
+    <t>dialogue</t>
+  </si>
+  <si>
+    <t>Grammar police chief</t>
   </si>
 </sst>
 </file>
@@ -503,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EDE4036-C0FB-4C09-A3D4-2CFBF82B9520}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="124" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="105" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -519,18 +522,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -539,7 +542,7 @@
         <v>Narrator</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -548,7 +551,7 @@
         <v>Narrator</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -557,7 +560,7 @@
         <v>Narrator</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="56" x14ac:dyDescent="0.3">
@@ -566,7 +569,7 @@
         <v>Narrator</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -575,7 +578,7 @@
         <v>Narrator</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28" x14ac:dyDescent="0.3">
@@ -584,7 +587,7 @@
         <v>Narrator</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="28" x14ac:dyDescent="0.3">
@@ -593,7 +596,7 @@
         <v>Narrator</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="28" x14ac:dyDescent="0.3">
@@ -602,7 +605,7 @@
         <v>Narrator</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="42" x14ac:dyDescent="0.3">
@@ -611,7 +614,7 @@
         <v>Narrator</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -620,95 +623,95 @@
         <v>Narrator</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="str">
-        <f t="shared" ref="A16:A19" si="1">A15</f>
-        <v>Grammar Police chief</v>
+        <f t="shared" ref="A16:A17" si="1">A15</f>
+        <v>Grammar police chief</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>Grammar Police chief</v>
+        <v>Grammar police chief</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="56" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="str">
-        <f t="shared" ref="A19:A22" si="2">A19</f>
-        <v>Grammar Police chief</v>
+        <f t="shared" ref="A20:A22" si="2">A19</f>
+        <v>Grammar police chief</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="56" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>Grammar Police chief</v>
+        <v>Grammar police chief</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="28" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>Grammar Police chief</v>
+        <v>Grammar police chief</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>